<commit_message>
ryml works, server temporarily broken
</commit_message>
<xml_diff>
--- a/rpcs.xlsx
+++ b/rpcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rico\Documents\Visual Studio 2022\Projects\Valhalla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E6C692-B94A-4606-B20A-2490079CF922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854C55B6-15F9-491A-86B6-372BB26B0F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16005" yWindow="1740" windowWidth="16755" windowHeight="10275" activeTab="1" xr2:uid="{DF4641AB-0ED2-4526-94E1-8DE9BCE04204}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{DF4641AB-0ED2-4526-94E1-8DE9BCE04204}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId3"/>
+    <pivotCache cacheId="16" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="174">
   <si>
     <t>name</t>
   </si>
@@ -547,6 +547,21 @@
   </si>
   <si>
     <t>MusicVolume</t>
+  </si>
+  <si>
+    <t>isowner</t>
+  </si>
+  <si>
+    <t>partial</t>
+  </si>
+  <si>
+    <t>PickableItem</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -568,12 +583,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -588,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -599,6 +620,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,11 +643,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Rico" refreshedDate="44851.980916666667" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="131" xr:uid="{047AE783-D8FC-4F35-AAA1-1A023BDC083A}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Rico" refreshedDate="44855.540423842591" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="131" xr:uid="{78C04BC3-A41D-4FA0-81E5-32B808E2D996}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:D132" sheet="Sheet1"/>
+    <worksheetSource ref="A1:E132" sheet="Sheet1"/>
   </cacheSource>
-  <cacheFields count="4">
+  <cacheFields count="5">
     <cacheField name="name" numFmtId="0">
       <sharedItems count="118">
         <s v="Disconnect"/>
@@ -756,7 +781,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="class" numFmtId="0">
-      <sharedItems containsBlank="1" count="43">
+      <sharedItems containsBlank="1" count="42">
         <m/>
         <s v="ArmorStand"/>
         <s v="BaseAI"/>
@@ -772,8 +797,8 @@
         <s v="ItemStand"/>
         <s v="MusicLocation"/>
         <s v="MusicVolume"/>
-        <s v="Pick"/>
         <s v="Pickable"/>
+        <s v="PickableItem"/>
         <s v="Player"/>
         <s v="PrivateArea"/>
         <s v="Projectile"/>
@@ -799,7 +824,14 @@
         <s v="MineRock5"/>
         <s v="SEMan"/>
         <s v="Talker"/>
-        <s v="RPC_PlayMusic" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="isowner" numFmtId="0">
+      <sharedItems containsBlank="1" count="4">
+        <m/>
+        <b v="1"/>
+        <b v="0"/>
+        <s v="partial"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -818,17 +850,20 @@
     <x v="0"/>
     <m/>
     <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
@@ -836,776 +871,904 @@
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="5"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="6"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="7"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="8"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="9"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="10"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="11"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="12"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="13"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="14"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="15"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="16"/>
     <x v="0"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="17"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="18"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="19"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="20"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="21"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="22"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="23"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="24"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="25"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="26"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="27"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="28"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="29"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="30"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="31"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="32"/>
     <x v="1"/>
     <m/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="33"/>
     <x v="1"/>
     <s v="client"/>
     <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="34"/>
     <x v="2"/>
     <m/>
     <x v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="35"/>
     <x v="2"/>
     <m/>
     <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="36"/>
     <x v="2"/>
     <m/>
     <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="37"/>
     <x v="2"/>
     <m/>
     <x v="4"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="38"/>
     <x v="2"/>
     <m/>
     <x v="5"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="39"/>
     <x v="2"/>
     <m/>
     <x v="6"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="40"/>
     <x v="2"/>
     <m/>
     <x v="7"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="38"/>
     <x v="2"/>
     <m/>
     <x v="8"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="41"/>
     <x v="2"/>
     <m/>
     <x v="9"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="42"/>
     <x v="2"/>
     <m/>
     <x v="9"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="43"/>
     <x v="2"/>
     <m/>
     <x v="10"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="44"/>
     <x v="2"/>
     <m/>
     <x v="10"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="45"/>
     <x v="2"/>
     <m/>
     <x v="11"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="46"/>
     <x v="2"/>
     <m/>
     <x v="12"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="45"/>
     <x v="2"/>
     <m/>
     <x v="12"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="47"/>
     <x v="2"/>
     <m/>
     <x v="12"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="48"/>
     <x v="2"/>
     <m/>
     <x v="13"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="49"/>
     <x v="2"/>
     <m/>
     <x v="14"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="50"/>
     <x v="2"/>
     <m/>
     <x v="15"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="50"/>
     <x v="2"/>
     <m/>
     <x v="16"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="51"/>
     <x v="2"/>
     <m/>
     <x v="17"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="52"/>
     <x v="2"/>
     <m/>
     <x v="18"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="53"/>
     <x v="2"/>
     <m/>
     <x v="19"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="54"/>
     <x v="2"/>
     <m/>
     <x v="20"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="55"/>
     <x v="2"/>
     <m/>
     <x v="20"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="56"/>
     <x v="2"/>
     <m/>
     <x v="20"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="38"/>
     <x v="2"/>
     <m/>
     <x v="21"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="57"/>
     <x v="2"/>
     <m/>
     <x v="21"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="58"/>
     <x v="2"/>
     <m/>
     <x v="22"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="59"/>
     <x v="2"/>
     <m/>
     <x v="23"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="60"/>
     <x v="2"/>
     <m/>
     <x v="23"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="45"/>
     <x v="2"/>
     <m/>
     <x v="24"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="61"/>
     <x v="2"/>
     <m/>
     <x v="24"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="62"/>
     <x v="2"/>
     <m/>
     <x v="25"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="63"/>
     <x v="2"/>
     <m/>
     <x v="25"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="64"/>
     <x v="2"/>
     <m/>
     <x v="25"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="65"/>
     <x v="2"/>
     <m/>
     <x v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="66"/>
     <x v="2"/>
     <m/>
     <x v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="67"/>
     <x v="2"/>
     <m/>
     <x v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="68"/>
     <x v="2"/>
     <m/>
     <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="69"/>
     <x v="2"/>
     <m/>
     <x v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="70"/>
     <x v="2"/>
     <m/>
     <x v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="71"/>
     <x v="2"/>
     <m/>
     <x v="4"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="72"/>
     <x v="2"/>
     <m/>
     <x v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="73"/>
     <x v="2"/>
     <m/>
     <x v="26"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="74"/>
     <x v="2"/>
     <m/>
     <x v="26"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="75"/>
     <x v="2"/>
     <m/>
     <x v="26"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="76"/>
     <x v="2"/>
     <m/>
     <x v="26"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="77"/>
     <x v="2"/>
     <m/>
     <x v="5"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="78"/>
     <x v="2"/>
     <m/>
     <x v="5"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="69"/>
     <x v="2"/>
     <m/>
     <x v="6"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="79"/>
     <x v="2"/>
     <m/>
     <x v="27"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="78"/>
     <x v="2"/>
     <m/>
     <x v="7"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="80"/>
     <x v="2"/>
     <m/>
     <x v="28"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="81"/>
     <x v="2"/>
     <m/>
     <x v="10"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="82"/>
     <x v="2"/>
     <m/>
     <x v="10"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="83"/>
     <x v="2"/>
     <m/>
     <x v="29"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="84"/>
     <x v="2"/>
     <m/>
     <x v="30"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="85"/>
     <x v="2"/>
     <m/>
-    <x v="16"/>
+    <x v="15"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="86"/>
     <x v="2"/>
     <m/>
     <x v="17"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="87"/>
     <x v="2"/>
     <m/>
     <x v="18"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="88"/>
     <x v="2"/>
     <m/>
     <x v="31"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="89"/>
     <x v="2"/>
     <m/>
     <x v="31"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="90"/>
     <x v="2"/>
     <m/>
     <x v="31"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="91"/>
     <x v="2"/>
     <m/>
     <x v="31"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="92"/>
     <x v="2"/>
     <m/>
     <x v="20"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="88"/>
     <x v="2"/>
     <m/>
     <x v="32"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="89"/>
     <x v="2"/>
     <m/>
     <x v="32"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="90"/>
     <x v="2"/>
     <m/>
     <x v="32"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="93"/>
     <x v="2"/>
     <m/>
     <x v="21"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="94"/>
     <x v="2"/>
     <m/>
     <x v="22"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="95"/>
     <x v="2"/>
     <m/>
     <x v="22"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="96"/>
     <x v="2"/>
     <m/>
     <x v="22"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="97"/>
     <x v="2"/>
     <m/>
     <x v="33"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="98"/>
     <x v="2"/>
     <m/>
     <x v="34"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="69"/>
     <x v="2"/>
     <m/>
     <x v="23"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="69"/>
     <x v="2"/>
     <m/>
     <x v="35"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="99"/>
     <x v="2"/>
     <m/>
     <x v="25"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="100"/>
     <x v="2"/>
     <m/>
     <x v="25"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="101"/>
     <x v="2"/>
     <m/>
     <x v="36"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="102"/>
     <x v="2"/>
     <m/>
     <x v="37"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="103"/>
     <x v="2"/>
     <m/>
     <x v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="104"/>
     <x v="2"/>
     <m/>
     <x v="5"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="105"/>
     <x v="2"/>
     <m/>
     <x v="38"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="106"/>
     <x v="2"/>
     <m/>
     <x v="12"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="107"/>
     <x v="2"/>
     <m/>
     <x v="30"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="69"/>
     <x v="2"/>
     <m/>
     <x v="39"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="108"/>
     <x v="2"/>
     <m/>
     <x v="39"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="109"/>
     <x v="2"/>
     <m/>
     <x v="17"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="110"/>
     <x v="2"/>
     <m/>
     <x v="18"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="111"/>
     <x v="2"/>
     <m/>
     <x v="40"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="112"/>
     <x v="2"/>
     <m/>
     <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="113"/>
     <x v="2"/>
     <m/>
     <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="114"/>
     <x v="2"/>
     <m/>
     <x v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="115"/>
     <x v="2"/>
     <m/>
     <x v="17"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="116"/>
     <x v="2"/>
     <m/>
     <x v="31"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="117"/>
     <x v="2"/>
     <m/>
     <x v="41"/>
+    <x v="2"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B49A818E-00B2-42AB-9BF3-EB4C60274751}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:A179" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73174B25-CE95-49FE-9ADA-C43547A5ECAD}" name="PivotTable2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:A137" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
       <items count="119">
         <item x="38"/>
@@ -1739,7 +1902,7 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="44">
+      <items count="43">
         <item x="1"/>
         <item x="2"/>
         <item x="37"/>
@@ -1762,11 +1925,9 @@
         <item x="39"/>
         <item x="13"/>
         <item x="15"/>
-        <item x="16"/>
         <item x="17"/>
         <item x="18"/>
         <item x="19"/>
-        <item m="1" x="42"/>
         <item x="31"/>
         <item x="40"/>
         <item x="20"/>
@@ -1783,16 +1944,27 @@
         <item x="36"/>
         <item x="0"/>
         <item x="14"/>
+        <item x="16"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item sd="0" x="2"/>
+        <item x="1"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="3">
+  <rowFields count="4">
     <field x="1"/>
+    <field x="4"/>
     <field x="3"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="178">
+  <rowItems count="136">
     <i>
       <x/>
     </i>
@@ -1800,528 +1972,402 @@
       <x/>
     </i>
     <i r="2">
-      <x v="70"/>
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="42"/>
     </i>
     <i r="2">
-      <x v="71"/>
+      <x v="21"/>
+    </i>
+    <i r="3">
+      <x v="89"/>
     </i>
     <i r="2">
-      <x v="72"/>
+      <x v="34"/>
+    </i>
+    <i r="3">
+      <x v="30"/>
     </i>
     <i r="2">
-      <x v="76"/>
-    </i>
-    <i r="2">
-      <x v="77"/>
-    </i>
-    <i r="2">
-      <x v="78"/>
+      <x v="40"/>
+    </i>
+    <i r="3">
+      <x v="74"/>
     </i>
     <i r="1">
       <x v="1"/>
     </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="70"/>
+    </i>
+    <i r="3">
+      <x v="71"/>
+    </i>
+    <i r="3">
+      <x v="72"/>
+    </i>
+    <i r="3">
+      <x v="76"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="3">
+      <x v="88"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
+    <i r="3">
+      <x v="16"/>
+    </i>
+    <i r="3">
+      <x v="31"/>
+    </i>
+    <i r="3">
+      <x v="79"/>
+    </i>
+    <i r="3">
+      <x v="94"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="3">
+      <x v="60"/>
+    </i>
+    <i r="3">
+      <x v="64"/>
+    </i>
     <i r="2">
       <x v="6"/>
     </i>
+    <i r="3">
+      <x/>
+    </i>
     <i r="2">
-      <x v="42"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
+      <x v="7"/>
+    </i>
+    <i r="3">
+      <x v="16"/>
     </i>
     <i r="2">
-      <x v="88"/>
+      <x v="9"/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="106"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="14"/>
+    </i>
+    <i r="3">
+      <x v="75"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i r="3">
+      <x v="61"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i r="3">
+      <x v="18"/>
+    </i>
+    <i r="3">
+      <x v="23"/>
+    </i>
+    <i r="3">
+      <x v="61"/>
+    </i>
+    <i r="2">
+      <x v="17"/>
+    </i>
+    <i r="3">
+      <x v="36"/>
+    </i>
+    <i r="2">
+      <x v="18"/>
+    </i>
+    <i r="3">
+      <x v="33"/>
+    </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
+    <i r="3">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x v="20"/>
+    </i>
+    <i r="3">
+      <x v="90"/>
+    </i>
+    <i r="2">
+      <x v="21"/>
+    </i>
+    <i r="3">
+      <x v="46"/>
+    </i>
+    <i r="2">
+      <x v="22"/>
+    </i>
+    <i r="3">
+      <x v="37"/>
+    </i>
+    <i r="2">
+      <x v="23"/>
+    </i>
+    <i r="3">
+      <x v="107"/>
+    </i>
+    <i r="3">
+      <x v="108"/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i r="3">
+      <x v="14"/>
+    </i>
+    <i r="3">
+      <x v="53"/>
+    </i>
+    <i r="3">
+      <x v="57"/>
+    </i>
+    <i r="3">
+      <x v="58"/>
+    </i>
+    <i r="2">
+      <x v="26"/>
+    </i>
+    <i r="3">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="28"/>
+    </i>
+    <i r="3">
+      <x v="53"/>
+    </i>
+    <i r="3">
+      <x v="58"/>
+    </i>
+    <i r="2">
+      <x v="29"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="3"/>
+    </i>
+    <i r="3">
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="31"/>
+    </i>
+    <i r="3">
+      <x v="4"/>
+    </i>
+    <i r="3">
+      <x v="87"/>
+    </i>
+    <i r="2">
+      <x v="32"/>
+    </i>
+    <i r="3">
+      <x v="93"/>
+    </i>
+    <i r="2">
+      <x v="33"/>
+    </i>
+    <i r="3">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="34"/>
+    </i>
+    <i r="3">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x v="35"/>
+    </i>
+    <i r="3">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x v="36"/>
+    </i>
+    <i r="3">
+      <x v="61"/>
+    </i>
+    <i r="2">
+      <x v="37"/>
+    </i>
+    <i r="3">
+      <x v="113"/>
+    </i>
+    <i r="3">
+      <x v="115"/>
+    </i>
+    <i r="3">
+      <x v="116"/>
+    </i>
+    <i r="2">
+      <x v="41"/>
+    </i>
+    <i r="3">
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="1"/>
     </i>
     <i r="1">
       <x v="3"/>
     </i>
     <i r="2">
-      <x v="26"/>
+      <x v="39"/>
+    </i>
+    <i r="3">
+      <x v="11"/>
+    </i>
+    <i r="3">
+      <x v="17"/>
+    </i>
+    <i r="3">
+      <x v="19"/>
+    </i>
+    <i r="3">
+      <x v="21"/>
+    </i>
+    <i r="3">
+      <x v="22"/>
+    </i>
+    <i r="3">
+      <x v="29"/>
+    </i>
+    <i r="3">
+      <x v="35"/>
+    </i>
+    <i r="3">
+      <x v="48"/>
+    </i>
+    <i r="3">
+      <x v="50"/>
+    </i>
+    <i r="3">
+      <x v="56"/>
+    </i>
+    <i r="3">
+      <x v="65"/>
+    </i>
+    <i r="3">
+      <x v="85"/>
+    </i>
+    <i r="3">
+      <x v="86"/>
+    </i>
+    <i r="3">
+      <x v="98"/>
+    </i>
+    <i r="3">
+      <x v="99"/>
+    </i>
+    <i r="3">
+      <x v="100"/>
+    </i>
+    <i r="3">
+      <x v="101"/>
+    </i>
+    <i>
+      <x v="2"/>
     </i>
     <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="16"/>
-    </i>
-    <i r="2">
-      <x v="31"/>
-    </i>
-    <i r="2">
-      <x v="66"/>
-    </i>
-    <i r="2">
-      <x v="79"/>
-    </i>
-    <i r="2">
-      <x v="94"/>
-    </i>
-    <i r="2">
-      <x v="102"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="2">
-      <x v="44"/>
-    </i>
-    <i r="2">
-      <x v="60"/>
-    </i>
-    <i r="2">
-      <x v="64"/>
-    </i>
-    <i r="2">
-      <x v="105"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="55"/>
-    </i>
-    <i r="2">
-      <x v="92"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="2">
-      <x v="15"/>
-    </i>
-    <i r="2">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="2">
-      <x v="110"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="106"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="47"/>
-    </i>
-    <i r="2">
-      <x v="62"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
+      <x v="3"/>
     </i>
     <i r="2">
       <x v="39"/>
     </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="2">
-      <x v="103"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="2">
-      <x v="68"/>
-    </i>
-    <i r="2">
-      <x v="69"/>
-    </i>
-    <i r="2">
-      <x v="73"/>
-    </i>
-    <i r="2">
-      <x v="75"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="2">
-      <x v="61"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="2">
-      <x v="18"/>
-    </i>
-    <i r="2">
-      <x v="23"/>
-    </i>
-    <i r="2">
-      <x v="61"/>
-    </i>
-    <i r="2">
-      <x v="96"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="2">
-      <x v="36"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="2">
-      <x v="32"/>
-    </i>
-    <i r="2">
-      <x v="33"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="2">
-      <x v="16"/>
-    </i>
-    <i r="2">
-      <x v="84"/>
-    </i>
-    <i r="1">
+    <i r="3">
+      <x v="9"/>
+    </i>
+    <i r="3">
+      <x v="10"/>
+    </i>
+    <i r="3">
+      <x v="12"/>
+    </i>
+    <i r="3">
       <x v="20"/>
     </i>
-    <i r="2">
-      <x v="90"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
-    </i>
-    <i r="2">
-      <x v="46"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i r="2">
-      <x v="46"/>
-    </i>
-    <i r="2">
-      <x v="89"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
-    </i>
-    <i r="2">
-      <x v="37"/>
-    </i>
-    <i r="2">
-      <x v="40"/>
-    </i>
-    <i r="2">
-      <x v="43"/>
-    </i>
-    <i r="2">
-      <x v="111"/>
-    </i>
-    <i r="1">
-      <x v="24"/>
-    </i>
-    <i r="2">
-      <x v="27"/>
-    </i>
-    <i r="2">
-      <x v="107"/>
-    </i>
-    <i r="2">
-      <x v="108"/>
-    </i>
-    <i r="1">
+    <i r="3">
       <x v="25"/>
     </i>
-    <i r="2">
-      <x v="41"/>
-    </i>
-    <i r="1">
-      <x v="27"/>
-    </i>
-    <i r="2">
-      <x v="14"/>
-    </i>
-    <i r="2">
-      <x v="53"/>
-    </i>
-    <i r="2">
-      <x v="57"/>
-    </i>
-    <i r="2">
-      <x v="58"/>
-    </i>
-    <i r="2">
-      <x v="63"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="29"/>
-    </i>
-    <i r="2">
-      <x v="8"/>
-    </i>
-    <i r="2">
-      <x v="28"/>
-    </i>
-    <i r="2">
-      <x v="80"/>
-    </i>
-    <i r="2">
-      <x v="104"/>
-    </i>
-    <i r="1">
-      <x v="30"/>
-    </i>
-    <i r="2">
-      <x v="53"/>
-    </i>
-    <i r="2">
-      <x v="58"/>
-    </i>
-    <i r="2">
-      <x v="63"/>
-    </i>
-    <i r="1">
-      <x v="31"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x v="24"/>
-    </i>
-    <i r="1">
-      <x v="32"/>
-    </i>
-    <i r="2">
-      <x v="82"/>
-    </i>
-    <i r="1">
-      <x v="33"/>
-    </i>
-    <i r="2">
-      <x v="4"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="2">
-      <x v="87"/>
-    </i>
-    <i r="2">
-      <x v="91"/>
-    </i>
-    <i r="1">
+    <i r="3">
       <x v="34"/>
     </i>
-    <i r="2">
-      <x v="93"/>
-    </i>
-    <i r="1">
-      <x v="35"/>
-    </i>
-    <i r="2">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="36"/>
-    </i>
-    <i r="2">
-      <x v="16"/>
-    </i>
-    <i r="2">
-      <x v="30"/>
-    </i>
-    <i r="2">
-      <x v="97"/>
-    </i>
-    <i r="1">
-      <x v="37"/>
-    </i>
-    <i r="2">
-      <x v="16"/>
-    </i>
-    <i r="1">
+    <i r="3">
       <x v="38"/>
     </i>
-    <i r="2">
-      <x v="59"/>
-    </i>
-    <i r="2">
-      <x v="61"/>
-    </i>
-    <i r="1">
-      <x v="39"/>
-    </i>
-    <i r="2">
-      <x v="112"/>
-    </i>
-    <i r="2">
-      <x v="113"/>
-    </i>
-    <i r="2">
-      <x v="114"/>
-    </i>
-    <i r="2">
-      <x v="115"/>
-    </i>
-    <i r="2">
-      <x v="116"/>
-    </i>
-    <i r="1">
-      <x v="40"/>
-    </i>
-    <i r="2">
-      <x v="95"/>
-    </i>
-    <i r="1">
-      <x v="42"/>
-    </i>
-    <i r="2">
-      <x v="74"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="41"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="17"/>
-    </i>
-    <i r="2">
-      <x v="19"/>
-    </i>
-    <i r="2">
-      <x v="21"/>
-    </i>
-    <i r="2">
-      <x v="22"/>
-    </i>
-    <i r="2">
-      <x v="29"/>
-    </i>
-    <i r="2">
-      <x v="35"/>
-    </i>
-    <i r="2">
-      <x v="48"/>
-    </i>
-    <i r="2">
-      <x v="50"/>
-    </i>
-    <i r="2">
-      <x v="56"/>
-    </i>
-    <i r="2">
-      <x v="65"/>
-    </i>
-    <i r="2">
-      <x v="85"/>
-    </i>
-    <i r="2">
-      <x v="86"/>
-    </i>
-    <i r="2">
-      <x v="98"/>
-    </i>
-    <i r="2">
-      <x v="99"/>
-    </i>
-    <i r="2">
-      <x v="100"/>
-    </i>
-    <i r="2">
-      <x v="101"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="41"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="20"/>
-    </i>
-    <i r="2">
-      <x v="25"/>
-    </i>
-    <i r="2">
-      <x v="34"/>
-    </i>
-    <i r="2">
-      <x v="38"/>
-    </i>
-    <i r="2">
+    <i r="3">
       <x v="45"/>
     </i>
-    <i r="2">
+    <i r="3">
       <x v="49"/>
     </i>
-    <i r="2">
+    <i r="3">
       <x v="51"/>
     </i>
-    <i r="2">
+    <i r="3">
       <x v="52"/>
     </i>
-    <i r="2">
+    <i r="3">
       <x v="54"/>
     </i>
-    <i r="2">
+    <i r="3">
       <x v="67"/>
     </i>
-    <i r="2">
+    <i r="3">
       <x v="81"/>
     </i>
-    <i r="2">
+    <i r="3">
       <x v="83"/>
     </i>
-    <i r="2">
+    <i r="3">
       <x v="109"/>
     </i>
-    <i r="2">
+    <i r="3">
       <x v="117"/>
     </i>
     <i t="grand">
@@ -2642,28 +2688,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5712C22C-3F48-4606-BB30-F52B8146841F}">
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>73</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -2923,7 +2973,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2931,7 +2981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2939,7 +2989,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2950,7 +3000,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -2960,8 +3010,11 @@
       <c r="D36" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -2971,8 +3024,11 @@
       <c r="D37" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -2982,8 +3038,11 @@
       <c r="D38" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2993,8 +3052,11 @@
       <c r="D39" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -3004,8 +3066,11 @@
       <c r="D40" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -3015,8 +3080,11 @@
       <c r="D41" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -3026,8 +3094,11 @@
       <c r="D42" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -3037,8 +3108,11 @@
       <c r="D43" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -3048,8 +3122,11 @@
       <c r="D44" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -3059,8 +3136,11 @@
       <c r="D45" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -3070,8 +3150,11 @@
       <c r="D46" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -3081,8 +3164,11 @@
       <c r="D47" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -3092,8 +3178,11 @@
       <c r="D48" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -3103,8 +3192,11 @@
       <c r="D49" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -3114,8 +3206,11 @@
       <c r="D50" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -3125,8 +3220,11 @@
       <c r="D51" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -3136,8 +3234,11 @@
       <c r="D52" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -3147,8 +3248,11 @@
       <c r="D53" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -3156,10 +3260,13 @@
         <v>20</v>
       </c>
       <c r="D54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -3167,10 +3274,13 @@
         <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -3180,8 +3290,11 @@
       <c r="D56" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -3191,8 +3304,11 @@
       <c r="D57" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -3202,8 +3318,11 @@
       <c r="D58" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -3213,8 +3332,11 @@
       <c r="D59" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -3224,8 +3346,11 @@
       <c r="D60" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -3235,8 +3360,11 @@
       <c r="D61" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>46</v>
       </c>
@@ -3246,8 +3374,11 @@
       <c r="D62" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -3257,8 +3388,11 @@
       <c r="D63" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>66</v>
       </c>
@@ -3268,8 +3402,11 @@
       <c r="D64" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -3279,8 +3416,11 @@
       <c r="D65" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -3290,8 +3430,11 @@
       <c r="D66" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>53</v>
       </c>
@@ -3301,8 +3444,11 @@
       <c r="D67" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -3312,8 +3458,11 @@
       <c r="D68" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -3323,8 +3472,11 @@
       <c r="D69" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -3334,8 +3486,11 @@
       <c r="D70" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -3345,8 +3500,11 @@
       <c r="D71" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -3356,8 +3514,11 @@
       <c r="D72" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -3367,8 +3528,11 @@
       <c r="D73" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -3378,8 +3542,11 @@
       <c r="D74" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -3389,8 +3556,11 @@
       <c r="D75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -3400,8 +3570,11 @@
       <c r="D76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -3411,8 +3584,11 @@
       <c r="D77" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -3422,8 +3598,11 @@
       <c r="D78" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -3433,8 +3612,11 @@
       <c r="D79" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>84</v>
       </c>
@@ -3444,8 +3626,11 @@
       <c r="D80" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -3455,8 +3640,11 @@
       <c r="D81" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>86</v>
       </c>
@@ -3466,8 +3654,11 @@
       <c r="D82" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -3477,8 +3668,11 @@
       <c r="D83" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -3488,8 +3682,11 @@
       <c r="D84" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>89</v>
       </c>
@@ -3499,8 +3696,11 @@
       <c r="D85" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -3510,8 +3710,11 @@
       <c r="D86" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -3521,8 +3724,11 @@
       <c r="D87" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -3532,8 +3738,11 @@
       <c r="D88" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -3543,8 +3752,11 @@
       <c r="D89" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -3554,8 +3766,11 @@
       <c r="D90" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -3565,8 +3780,11 @@
       <c r="D91" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -3576,8 +3794,11 @@
       <c r="D92" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>103</v>
       </c>
@@ -3587,8 +3808,11 @@
       <c r="D93" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>104</v>
       </c>
@@ -3598,8 +3822,11 @@
       <c r="D94" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>106</v>
       </c>
@@ -3609,8 +3836,11 @@
       <c r="D95" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>109</v>
       </c>
@@ -3620,8 +3850,11 @@
       <c r="D96" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>110</v>
       </c>
@@ -3631,8 +3864,11 @@
       <c r="D97" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>111</v>
       </c>
@@ -3642,8 +3878,11 @@
       <c r="D98" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>112</v>
       </c>
@@ -3653,8 +3892,11 @@
       <c r="D99" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>113</v>
       </c>
@@ -3664,8 +3906,11 @@
       <c r="D100" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -3675,8 +3920,11 @@
       <c r="D101" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>110</v>
       </c>
@@ -3686,8 +3934,11 @@
       <c r="D102" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>111</v>
       </c>
@@ -3697,8 +3948,11 @@
       <c r="D103" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>112</v>
       </c>
@@ -3708,8 +3962,11 @@
       <c r="D104" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>118</v>
       </c>
@@ -3719,8 +3976,11 @@
       <c r="D105" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>121</v>
       </c>
@@ -3730,8 +3990,11 @@
       <c r="D106" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>122</v>
       </c>
@@ -3741,8 +4004,11 @@
       <c r="D107" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>123</v>
       </c>
@@ -3752,8 +4018,11 @@
       <c r="D108" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>124</v>
       </c>
@@ -3763,8 +4032,11 @@
       <c r="D109" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -3774,8 +4046,11 @@
       <c r="D110" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>80</v>
       </c>
@@ -3785,8 +4060,11 @@
       <c r="D111" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>80</v>
       </c>
@@ -3795,6 +4073,9 @@
       </c>
       <c r="D112" t="s">
         <v>129</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3807,6 +4088,9 @@
       <c r="D113" t="s">
         <v>130</v>
       </c>
+      <c r="E113" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
@@ -3818,6 +4102,9 @@
       <c r="D114" t="s">
         <v>130</v>
       </c>
+      <c r="E114" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -3829,6 +4116,9 @@
       <c r="D115" t="s">
         <v>131</v>
       </c>
+      <c r="E115" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
@@ -3840,8 +4130,8 @@
       <c r="D116" t="s">
         <v>135</v>
       </c>
-      <c r="E116">
-        <v>2</v>
+      <c r="E116" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3854,6 +4144,9 @@
       <c r="D117" t="s">
         <v>75</v>
       </c>
+      <c r="E117" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
@@ -3865,6 +4158,9 @@
       <c r="D118" t="s">
         <v>90</v>
       </c>
+      <c r="E118" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
@@ -3876,6 +4172,9 @@
       <c r="D119" t="s">
         <v>140</v>
       </c>
+      <c r="E119" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
@@ -3887,6 +4186,9 @@
       <c r="D120" t="s">
         <v>141</v>
       </c>
+      <c r="E120" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
@@ -3898,6 +4200,9 @@
       <c r="D121" t="s">
         <v>102</v>
       </c>
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
@@ -3909,6 +4214,9 @@
       <c r="D122" t="s">
         <v>145</v>
       </c>
+      <c r="E122" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -3920,6 +4228,9 @@
       <c r="D123" t="s">
         <v>145</v>
       </c>
+      <c r="E123" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
@@ -3931,6 +4242,9 @@
       <c r="D124" t="s">
         <v>107</v>
       </c>
+      <c r="E124" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -3942,6 +4256,9 @@
       <c r="D125" t="s">
         <v>108</v>
       </c>
+      <c r="E125" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -3953,6 +4270,9 @@
       <c r="D126" t="s">
         <v>149</v>
       </c>
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
@@ -3964,6 +4284,9 @@
       <c r="D127" t="s">
         <v>74</v>
       </c>
+      <c r="E127" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
@@ -3975,6 +4298,9 @@
       <c r="D128" t="s">
         <v>152</v>
       </c>
+      <c r="E128" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
@@ -3986,6 +4312,9 @@
       <c r="D129" t="s">
         <v>75</v>
       </c>
+      <c r="E129" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
@@ -3997,6 +4326,9 @@
       <c r="D130" t="s">
         <v>107</v>
       </c>
+      <c r="E130" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -4008,6 +4340,9 @@
       <c r="D131" t="s">
         <v>114</v>
       </c>
+      <c r="E131" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
@@ -4019,8 +4354,8 @@
       <c r="D132" t="s">
         <v>156</v>
       </c>
-      <c r="E132">
-        <v>3</v>
+      <c r="E132" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4031,15 +4366,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623EDF76-DB11-4620-8721-1BF802DC5619}">
-  <dimension ref="A1:A179"/>
+  <dimension ref="A1:A137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132:A136"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -4054,886 +4389,676 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>41</v>
+      <c r="A5" s="6" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>42</v>
+      <c r="A7" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>150</v>
+      <c r="A9" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>152</v>
+      <c r="A10" s="4" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>43</v>
+      <c r="A11" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>151</v>
+      <c r="A12" s="3" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>158</v>
+      <c r="A15" s="6" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>44</v>
+      <c r="A16" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>75</v>
+      <c r="A17" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>81</v>
+      <c r="A18" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>137</v>
+      <c r="A20" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>153</v>
+      <c r="A22" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>90</v>
+      <c r="A30" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>46</v>
+      <c r="A31" s="6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>88</v>
+      <c r="A33" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>91</v>
+      <c r="A35" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>80</v>
+      <c r="A37" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>93</v>
+      <c r="A38" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>92</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>94</v>
+      <c r="A40" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>48</v>
+      <c r="A42" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>159</v>
+      <c r="A43" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>46</v>
+      <c r="A44" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>160</v>
+      <c r="A45" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>50</v>
+      <c r="A46" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>49</v>
+      <c r="A47" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>96</v>
+      <c r="A48" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>140</v>
+      <c r="A50" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>97</v>
+      <c r="A52" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>51</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>52</v>
+      <c r="A54" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>98</v>
+      <c r="A56" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>161</v>
+      <c r="A57" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>53</v>
+      <c r="A58" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>141</v>
+      <c r="A59" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>55</v>
+      <c r="A60" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>53</v>
+      <c r="A62" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>142</v>
+      <c r="A63" s="6" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>100</v>
+      <c r="A64" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>101</v>
+      <c r="A65" s="6" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>102</v>
+      <c r="A66" s="6" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>103</v>
+      <c r="A67" s="6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>143</v>
+      <c r="A68" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>145</v>
+      <c r="A69" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>80</v>
+      <c r="A70" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>162</v>
+      <c r="A72" s="6" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>56</v>
+      <c r="A73" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>58</v>
+      <c r="A74" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>58</v>
+      <c r="A75" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>105</v>
+      <c r="A76" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>58</v>
+      <c r="A77" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>107</v>
+      <c r="A79" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>154</v>
+      <c r="A80" s="6" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>146</v>
+      <c r="A82" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>108</v>
+      <c r="A84" s="6" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>109</v>
+      <c r="A86" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>163</v>
+      <c r="A88" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>61</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>114</v>
+      <c r="A90" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>111</v>
+      <c r="A92" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>113</v>
+      <c r="A93" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>110</v>
+      <c r="A94" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
-        <v>149</v>
+      <c r="A96" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>148</v>
+      <c r="A97" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>116</v>
+        <v>167</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>63</v>
+      <c r="A100" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
-        <v>115</v>
+      <c r="A101" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>62</v>
+      <c r="A102" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>117</v>
+      <c r="A103" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>111</v>
+      <c r="A104" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
-        <v>110</v>
+      <c r="A105" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>112</v>
+      <c r="A106" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
-        <v>119</v>
+      <c r="A107" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
-        <v>46</v>
+      <c r="A108" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
-        <v>118</v>
+      <c r="A109" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
-        <v>65</v>
+      <c r="A110" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
-        <v>156</v>
+      <c r="A111" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
-        <v>157</v>
+      <c r="A112" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
-        <v>120</v>
+      <c r="A113" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
-        <v>66</v>
+      <c r="A114" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
-        <v>121</v>
+      <c r="A115" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
-        <v>122</v>
+      <c r="A116" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
-        <v>123</v>
+      <c r="A117" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>125</v>
+        <v>167</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>124</v>
+        <v>167</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>127</v>
+      <c r="A120" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
-        <v>126</v>
+      <c r="A121" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
-        <v>128</v>
+      <c r="A122" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
-        <v>80</v>
+      <c r="A123" s="6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
-        <v>67</v>
+      <c r="A124" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
-        <v>68</v>
+      <c r="A125" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
-        <v>129</v>
+      <c r="A126" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
-        <v>80</v>
+      <c r="A127" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="s">
-        <v>164</v>
+      <c r="A128" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="4" t="s">
-        <v>69</v>
+      <c r="A129" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="4" t="s">
-        <v>53</v>
+      <c r="A130" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
-        <v>130</v>
+      <c r="A131" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
-        <v>72</v>
+      <c r="A132" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="4" t="s">
-        <v>132</v>
+      <c r="A133" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="4" t="s">
-        <v>133</v>
+      <c r="A134" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="4" t="s">
-        <v>70</v>
+      <c r="A135" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="4" t="s">
-        <v>71</v>
+      <c r="A136" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="2" t="s">
+      <c r="A137" s="2" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>